<commit_message>
Final version of SPR, fixes to other posts.
</commit_message>
<xml_diff>
--- a/_posts/2024-08-25-the-depletion-of-the-strategic-petroleum-reserve/10621_crude_imports_1-15-24.xlsx
+++ b/_posts/2024-08-25-the-depletion-of-the-strategic-petroleum-reserve/10621_crude_imports_1-15-24.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmdavis\OneDrive\WTFIT\_posts\2024-08-25-the-depletion-of-the-strategic-petroleum-reserve\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0ccb503b6fdaa55a/Documents/What-are-we-doing/_posts/2024-08-25-the-depletion-of-the-strategic-petroleum-reserve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C6B648-8AD8-412B-8461-FA37DACBB74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{42C6B648-8AD8-412B-8461-FA37DACBB74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3225E933-D5BF-44C1-806A-2B36D14EC434}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -647,6 +647,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -673,10 +677,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4422,10 +4422,10 @@
   <dimension ref="B1:Z67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M54" sqref="M54"/>
+      <selection pane="bottomRight" activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -4440,7 +4440,7 @@
     <col min="10" max="10" width="16.42578125" customWidth="1"/>
     <col min="11" max="11" width="10.140625" customWidth="1"/>
     <col min="12" max="12" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="52"/>
+    <col min="13" max="13" width="8.85546875" style="42"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
@@ -4455,18 +4455,18 @@
   <sheetData>
     <row r="1" spans="2:26" ht="13.5" thickBot="1"/>
     <row r="2" spans="2:26" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="43"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="2:26" ht="33" customHeight="1">
       <c r="B3" s="21" t="s">
@@ -4499,10 +4499,10 @@
       <c r="K3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="51" t="s">
+      <c r="L3" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="53" t="s">
+      <c r="M3" s="43" t="s">
         <v>21</v>
       </c>
       <c r="P3" s="8"/>
@@ -4549,13 +4549,13 @@
         <f t="shared" ref="K4:K54" si="0">SUM(C4:J4)</f>
         <v>6256.1459999999997</v>
       </c>
-      <c r="L4" s="50">
+      <c r="L4" s="40">
         <f>(G4+H4)/K4</f>
         <v>0.21427041504466171</v>
       </c>
-      <c r="M4" s="52">
-        <f t="shared" ref="M4:M31" si="1">(I4+F4+C4+D4)/K4</f>
-        <v>0.48188661198124216</v>
+      <c r="M4" s="42">
+        <f>(I4+F4+C4)/K4</f>
+        <v>0.30047908089101505</v>
       </c>
       <c r="O4" s="7"/>
       <c r="P4" s="6"/>
@@ -4602,13 +4602,13 @@
         <f t="shared" si="0"/>
         <v>6112.183</v>
       </c>
-      <c r="L5" s="50">
-        <f t="shared" ref="L5:L54" si="2">(G5+H5)/K5</f>
+      <c r="L5" s="40">
+        <f t="shared" ref="L5:L54" si="1">(G5+H5)/K5</f>
         <v>0.17636595632035232</v>
       </c>
-      <c r="M5" s="52">
-        <f t="shared" si="1"/>
-        <v>0.53595024887180243</v>
+      <c r="M5" s="42">
+        <f t="shared" ref="M5:M54" si="2">(I5+F5+C5)/K5</f>
+        <v>0.37576263668807036</v>
       </c>
       <c r="O5" s="7"/>
       <c r="P5" s="6"/>
@@ -4655,13 +4655,13 @@
         <f t="shared" si="0"/>
         <v>6055.7129999999997</v>
       </c>
-      <c r="L6" s="50">
+      <c r="L6" s="40">
+        <f t="shared" si="1"/>
+        <v>0.15156877480818526</v>
+      </c>
+      <c r="M6" s="42">
         <f t="shared" si="2"/>
-        <v>0.15156877480818526</v>
-      </c>
-      <c r="M6" s="52">
-        <f t="shared" si="1"/>
-        <v>0.59667111040434051</v>
+        <v>0.48067023651880464</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="6"/>
@@ -4708,13 +4708,13 @@
         <f t="shared" si="0"/>
         <v>7312.5969999999998</v>
       </c>
-      <c r="L7" s="50">
+      <c r="L7" s="40">
+        <f t="shared" si="1"/>
+        <v>9.38685668032848E-2</v>
+      </c>
+      <c r="M7" s="42">
         <f t="shared" si="2"/>
-        <v>9.38685668032848E-2</v>
-      </c>
-      <c r="M7" s="52">
-        <f t="shared" si="1"/>
-        <v>0.69062304404303976</v>
+        <v>0.59488551057852646</v>
       </c>
       <c r="O7" s="7"/>
       <c r="P7" s="6"/>
@@ -4761,13 +4761,13 @@
         <f t="shared" si="0"/>
         <v>8807.2489999999998</v>
       </c>
-      <c r="L8" s="50">
+      <c r="L8" s="40">
+        <f t="shared" si="1"/>
+        <v>7.9066232827072341E-2</v>
+      </c>
+      <c r="M8" s="42">
         <f t="shared" si="2"/>
-        <v>7.9066232827072341E-2</v>
-      </c>
-      <c r="M8" s="52">
-        <f t="shared" si="1"/>
-        <v>0.69612429488481598</v>
+        <v>0.61773897842561287</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="7"/>
@@ -4815,13 +4815,13 @@
         <f t="shared" si="0"/>
         <v>8363.4110000000001</v>
       </c>
-      <c r="L9" s="50">
+      <c r="L9" s="40">
+        <f t="shared" si="1"/>
+        <v>9.3810766922730451E-2</v>
+      </c>
+      <c r="M9" s="42">
         <f t="shared" si="2"/>
-        <v>9.3810766922730451E-2</v>
-      </c>
-      <c r="M9" s="52">
-        <f t="shared" si="1"/>
-        <v>0.6812407043011518</v>
+        <v>0.60405915720272507</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="7"/>
@@ -4869,13 +4869,13 @@
         <f t="shared" si="0"/>
         <v>8456.1269999999986</v>
       </c>
-      <c r="L10" s="50">
+      <c r="L10" s="40">
+        <f t="shared" si="1"/>
+        <v>0.11550607033219819</v>
+      </c>
+      <c r="M10" s="42">
         <f t="shared" si="2"/>
-        <v>0.11550607033219819</v>
-      </c>
-      <c r="M10" s="52">
-        <f t="shared" si="1"/>
-        <v>0.65643479574041408</v>
+        <v>0.57482651336717161</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="7"/>
@@ -4923,13 +4923,13 @@
         <f t="shared" si="0"/>
         <v>6909.0240000000003</v>
       </c>
-      <c r="L11" s="50">
+      <c r="L11" s="40">
+        <f t="shared" si="1"/>
+        <v>0.14294435798746682</v>
+      </c>
+      <c r="M11" s="42">
         <f t="shared" si="2"/>
-        <v>0.14294435798746682</v>
-      </c>
-      <c r="M11" s="52">
-        <f t="shared" si="1"/>
-        <v>0.61839892291588505</v>
+        <v>0.54874465626403957</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="7"/>
@@ -4977,13 +4977,13 @@
         <f t="shared" si="0"/>
         <v>5995.6740000000009</v>
       </c>
-      <c r="L12" s="50">
+      <c r="L12" s="40">
+        <f t="shared" si="1"/>
+        <v>0.16172210163527903</v>
+      </c>
+      <c r="M12" s="42">
         <f t="shared" si="2"/>
-        <v>0.16172210163527903</v>
-      </c>
-      <c r="M12" s="52">
-        <f t="shared" si="1"/>
-        <v>0.55509505686933602</v>
+        <v>0.48736989369335282</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="7"/>
@@ -5031,13 +5031,13 @@
         <f t="shared" si="0"/>
         <v>5113.1589999999997</v>
       </c>
-      <c r="L13" s="50">
+      <c r="L13" s="40">
+        <f t="shared" si="1"/>
+        <v>0.22825126306457516</v>
+      </c>
+      <c r="M13" s="42">
         <f t="shared" si="2"/>
-        <v>0.22825126306457516</v>
-      </c>
-      <c r="M13" s="52">
-        <f t="shared" si="1"/>
-        <v>0.41925353778358943</v>
+        <v>0.33871154798823977</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="7"/>
@@ -5085,13 +5085,13 @@
         <f t="shared" si="0"/>
         <v>5051.3540000000003</v>
       </c>
-      <c r="L14" s="50">
+      <c r="L14" s="40">
+        <f t="shared" si="1"/>
+        <v>0.27193164446601842</v>
+      </c>
+      <c r="M14" s="42">
         <f t="shared" si="2"/>
-        <v>0.27193164446601842</v>
-      </c>
-      <c r="M14" s="52">
-        <f t="shared" si="1"/>
-        <v>0.36686044969329018</v>
+        <v>0.28331492902695005</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="7"/>
@@ -5139,13 +5139,13 @@
         <f t="shared" si="0"/>
         <v>5436.9830000000002</v>
       </c>
-      <c r="L15" s="50">
+      <c r="L15" s="40">
+        <f t="shared" si="1"/>
+        <v>0.25345048899362016</v>
+      </c>
+      <c r="M15" s="42">
         <f t="shared" si="2"/>
-        <v>0.25345048899362016</v>
-      </c>
-      <c r="M15" s="52">
-        <f t="shared" si="1"/>
-        <v>0.3769548295442528</v>
+        <v>0.27616345315039609</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="7"/>
@@ -5193,13 +5193,13 @@
         <f t="shared" si="0"/>
         <v>5067.143</v>
       </c>
-      <c r="L16" s="50">
+      <c r="L16" s="40">
+        <f t="shared" si="1"/>
+        <v>0.31297616822734231</v>
+      </c>
+      <c r="M16" s="42">
         <f t="shared" si="2"/>
-        <v>0.31297616822734231</v>
-      </c>
-      <c r="M16" s="52">
-        <f t="shared" si="1"/>
-        <v>0.35356590488959949</v>
+        <v>0.23420081098954579</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="7"/>
@@ -5247,13 +5247,13 @@
         <f t="shared" si="0"/>
         <v>6223.512999999999</v>
       </c>
-      <c r="L17" s="50">
+      <c r="L17" s="40">
+        <f t="shared" si="1"/>
+        <v>0.24185922002573149</v>
+      </c>
+      <c r="M17" s="42">
         <f t="shared" si="2"/>
-        <v>0.24185922002573149</v>
-      </c>
-      <c r="M17" s="52">
-        <f t="shared" si="1"/>
-        <v>0.44570405814208158</v>
+        <v>0.31827361813175298</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="7"/>
@@ -5301,13 +5301,13 @@
         <f t="shared" si="0"/>
         <v>6677.6960000000008</v>
       </c>
-      <c r="L18" s="50">
+      <c r="L18" s="40">
+        <f t="shared" si="1"/>
+        <v>0.22504663285061194</v>
+      </c>
+      <c r="M18" s="42">
         <f t="shared" si="2"/>
-        <v>0.22504663285061194</v>
-      </c>
-      <c r="M18" s="52">
-        <f t="shared" si="1"/>
-        <v>0.44750479806208593</v>
+        <v>0.32706071076011839</v>
       </c>
       <c r="N18" s="1"/>
       <c r="O18" s="7"/>
@@ -5355,13 +5355,13 @@
         <f t="shared" si="0"/>
         <v>7402.02</v>
       </c>
-      <c r="L19" s="50">
+      <c r="L19" s="40">
+        <f t="shared" si="1"/>
+        <v>0.23591978946287631</v>
+      </c>
+      <c r="M19" s="42">
         <f t="shared" si="2"/>
-        <v>0.23591978946287631</v>
-      </c>
-      <c r="M19" s="52">
-        <f t="shared" si="1"/>
-        <v>0.43271417802167511</v>
+        <v>0.32543359785572046</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="7"/>
@@ -5409,13 +5409,13 @@
         <f t="shared" si="0"/>
         <v>8060.5460000000003</v>
       </c>
-      <c r="L20" s="50">
+      <c r="L20" s="40">
+        <f t="shared" si="1"/>
+        <v>0.21070570157406207</v>
+      </c>
+      <c r="M20" s="42">
         <f t="shared" si="2"/>
-        <v>0.21070570157406207</v>
-      </c>
-      <c r="M20" s="52">
-        <f t="shared" si="1"/>
-        <v>0.46377329773938392</v>
+        <v>0.35550197219890561</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="7"/>
@@ -5463,13 +5463,13 @@
         <f t="shared" si="0"/>
         <v>8017.5220000000008</v>
       </c>
-      <c r="L21" s="50">
+      <c r="L21" s="40">
+        <f t="shared" si="1"/>
+        <v>0.21065236864956524</v>
+      </c>
+      <c r="M21" s="42">
         <f t="shared" si="2"/>
-        <v>0.21065236864956524</v>
-      </c>
-      <c r="M21" s="52">
-        <f t="shared" si="1"/>
-        <v>0.47683199372574214</v>
+        <v>0.34903352931242343</v>
       </c>
       <c r="N21" s="1"/>
       <c r="O21" s="7"/>
@@ -5517,13 +5517,13 @@
         <f t="shared" si="0"/>
         <v>7626.746000000001</v>
       </c>
-      <c r="L22" s="50">
+      <c r="L22" s="40">
+        <f t="shared" si="1"/>
+        <v>0.24119329527953334</v>
+      </c>
+      <c r="M22" s="42">
         <f t="shared" si="2"/>
-        <v>0.24119329527953334</v>
-      </c>
-      <c r="M22" s="52">
-        <f t="shared" si="1"/>
-        <v>0.54033555070537287</v>
+        <v>0.4046421632502249</v>
       </c>
       <c r="N22" s="1"/>
       <c r="O22" s="7"/>
@@ -5571,13 +5571,13 @@
         <f t="shared" si="0"/>
         <v>7887.6959999999999</v>
       </c>
-      <c r="L23" s="50">
+      <c r="L23" s="40">
+        <f t="shared" si="1"/>
+        <v>0.24078628283848669</v>
+      </c>
+      <c r="M23" s="42">
         <f t="shared" si="2"/>
-        <v>0.24078628283848669</v>
-      </c>
-      <c r="M23" s="52">
-        <f t="shared" si="1"/>
-        <v>0.5210331381939669</v>
+        <v>0.37272823394816434</v>
       </c>
       <c r="N23" s="1"/>
       <c r="O23" s="7"/>
@@ -5625,13 +5625,13 @@
         <f t="shared" si="0"/>
         <v>8620.4229999999989</v>
       </c>
-      <c r="L24" s="50">
+      <c r="L24" s="40">
+        <f t="shared" si="1"/>
+        <v>0.24359651492739973</v>
+      </c>
+      <c r="M24" s="42">
         <f t="shared" si="2"/>
-        <v>0.24359651492739973</v>
-      </c>
-      <c r="M24" s="52">
-        <f t="shared" si="1"/>
-        <v>0.50208800658621977</v>
+        <v>0.35123659245027772</v>
       </c>
       <c r="N24" s="1"/>
       <c r="O24" s="7"/>
@@ -5679,13 +5679,13 @@
         <f t="shared" si="0"/>
         <v>8996.2219999999998</v>
       </c>
-      <c r="L25" s="50">
+      <c r="L25" s="40">
+        <f t="shared" si="1"/>
+        <v>0.25077526988551418</v>
+      </c>
+      <c r="M25" s="42">
         <f t="shared" si="2"/>
-        <v>0.25077526988551418</v>
-      </c>
-      <c r="M25" s="52">
-        <f t="shared" si="1"/>
-        <v>0.47544502570078861</v>
+        <v>0.32719156997237286</v>
       </c>
       <c r="N25" s="1"/>
       <c r="O25" s="7"/>
@@ -5733,13 +5733,13 @@
         <f t="shared" si="0"/>
         <v>8834.9389999999985</v>
       </c>
-      <c r="L26" s="50">
+      <c r="L26" s="40">
+        <f t="shared" si="1"/>
+        <v>0.27161681591689546</v>
+      </c>
+      <c r="M26" s="42">
         <f t="shared" si="2"/>
-        <v>0.27161681591689546</v>
-      </c>
-      <c r="M26" s="52">
-        <f t="shared" si="1"/>
-        <v>0.45574361068027752</v>
+        <v>0.28819712280978965</v>
       </c>
       <c r="N26" s="1"/>
       <c r="O26" s="7"/>
@@ -5787,13 +5787,13 @@
         <f t="shared" si="0"/>
         <v>9478.4920000000002</v>
       </c>
-      <c r="L27" s="50">
+      <c r="L27" s="40">
+        <f t="shared" si="1"/>
+        <v>0.28148486067192963</v>
+      </c>
+      <c r="M27" s="42">
         <f t="shared" si="2"/>
-        <v>0.28148486067192963</v>
-      </c>
-      <c r="M27" s="52">
-        <f t="shared" si="1"/>
-        <v>0.4468358468836604</v>
+        <v>0.27001615868853407</v>
       </c>
       <c r="N27" s="1"/>
       <c r="O27" s="7"/>
@@ -5841,13 +5841,13 @@
         <f t="shared" si="0"/>
         <v>10161.563</v>
       </c>
-      <c r="L28" s="50">
+      <c r="L28" s="40">
+        <f t="shared" si="1"/>
+        <v>0.29016461345562683</v>
+      </c>
+      <c r="M28" s="42">
         <f t="shared" si="2"/>
-        <v>0.29016461345562683</v>
-      </c>
-      <c r="M28" s="52">
-        <f t="shared" si="1"/>
-        <v>0.44209576814118062</v>
+        <v>0.26762821821800442</v>
       </c>
       <c r="N28" s="1"/>
       <c r="O28" s="7"/>
@@ -5895,13 +5895,13 @@
         <f t="shared" si="0"/>
         <v>10708.072</v>
       </c>
-      <c r="L29" s="50">
+      <c r="L29" s="40">
+        <f t="shared" si="1"/>
+        <v>0.27545294801902709</v>
+      </c>
+      <c r="M29" s="42">
         <f t="shared" si="2"/>
-        <v>0.27545294801902709</v>
-      </c>
-      <c r="M29" s="52">
-        <f t="shared" si="1"/>
-        <v>0.42896807193675951</v>
+        <v>0.26843982744979672</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="7"/>
@@ -5949,13 +5949,13 @@
         <f t="shared" si="0"/>
         <v>10852.256000000001</v>
       </c>
-      <c r="L30" s="50">
+      <c r="L30" s="40">
+        <f t="shared" si="1"/>
+        <v>0.26388448632247524</v>
+      </c>
+      <c r="M30" s="42">
         <f t="shared" si="2"/>
-        <v>0.26388448632247524</v>
-      </c>
-      <c r="M30" s="52">
-        <f t="shared" si="1"/>
-        <v>0.39777968746774856</v>
+        <v>0.26024174144067369</v>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="7"/>
@@ -6003,13 +6003,13 @@
         <f t="shared" si="0"/>
         <v>11459.251</v>
       </c>
-      <c r="L31" s="50">
+      <c r="L31" s="40">
+        <f t="shared" si="1"/>
+        <v>0.27750024848919008</v>
+      </c>
+      <c r="M31" s="42">
         <f t="shared" si="2"/>
-        <v>0.27750024848919008</v>
-      </c>
-      <c r="M31" s="52">
-        <f t="shared" si="1"/>
-        <v>0.4062305642838262</v>
+        <v>0.27131083872759226</v>
       </c>
       <c r="N31" s="1"/>
       <c r="O31" s="7"/>
@@ -6057,13 +6057,13 @@
         <f t="shared" si="0"/>
         <v>11871.335999999999</v>
       </c>
-      <c r="L32" s="50">
+      <c r="L32" s="40">
+        <f t="shared" si="1"/>
+        <v>0.27531054634457319</v>
+      </c>
+      <c r="M32" s="42">
         <f t="shared" si="2"/>
-        <v>0.27531054634457319</v>
-      </c>
-      <c r="M32" s="52">
-        <f>(I32+F32+C32+D32)/K32</f>
-        <v>0.40633455240421129</v>
+        <v>0.27548036716339253</v>
       </c>
       <c r="N32" s="1"/>
       <c r="O32" s="7"/>
@@ -6111,13 +6111,13 @@
         <f t="shared" si="0"/>
         <v>11530.243000000002</v>
       </c>
-      <c r="L33" s="50">
+      <c r="L33" s="40">
+        <f t="shared" si="1"/>
+        <v>0.30505384838810418</v>
+      </c>
+      <c r="M33" s="42">
         <f t="shared" si="2"/>
-        <v>0.30505384838810418</v>
-      </c>
-      <c r="M33" s="52">
-        <f t="shared" ref="M33:M54" si="3">(I33+F33+C33+D33)/K33</f>
-        <v>0.37778943600754972</v>
+        <v>0.25652121989102911</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="7"/>
@@ -6165,13 +6165,13 @@
         <f t="shared" si="0"/>
         <v>12264.386999999999</v>
       </c>
-      <c r="L34" s="50">
+      <c r="L34" s="40">
+        <f t="shared" si="1"/>
+        <v>0.30131126814572962</v>
+      </c>
+      <c r="M34" s="42">
         <f t="shared" si="2"/>
-        <v>0.30131126814572962</v>
-      </c>
-      <c r="M34" s="52">
-        <f t="shared" si="3"/>
-        <v>0.40235260025633574</v>
+        <v>0.29013818627869459</v>
       </c>
       <c r="N34" s="1"/>
       <c r="O34" s="7"/>
@@ -6219,13 +6219,13 @@
         <f t="shared" si="0"/>
         <v>13145.094000000001</v>
       </c>
-      <c r="L35" s="50">
+      <c r="L35" s="40">
+        <f t="shared" si="1"/>
+        <v>0.28929386126869838</v>
+      </c>
+      <c r="M35" s="42">
         <f t="shared" si="2"/>
-        <v>0.28929386126869838</v>
-      </c>
-      <c r="M35" s="52">
-        <f t="shared" si="3"/>
-        <v>0.40643931492616175</v>
+        <v>0.28818287644044233</v>
       </c>
       <c r="N35" s="1"/>
       <c r="O35" s="7"/>
@@ -6273,13 +6273,13 @@
         <f t="shared" si="0"/>
         <v>13713.810000000001</v>
       </c>
-      <c r="L36" s="50">
+      <c r="L36" s="40">
+        <f t="shared" si="1"/>
+        <v>0.2802834514988905</v>
+      </c>
+      <c r="M36" s="42">
         <f t="shared" si="2"/>
-        <v>0.2802834514988905</v>
-      </c>
-      <c r="M36" s="52">
-        <f t="shared" si="3"/>
-        <v>0.39855474153426357</v>
+        <v>0.28704692569023482</v>
       </c>
       <c r="N36" s="1"/>
       <c r="O36" s="7"/>
@@ -6327,13 +6327,13 @@
         <f t="shared" si="0"/>
         <v>13707.073</v>
       </c>
-      <c r="L37" s="50">
+      <c r="L37" s="40">
+        <f t="shared" si="1"/>
+        <v>0.29606692836610704</v>
+      </c>
+      <c r="M37" s="42">
         <f t="shared" si="2"/>
-        <v>0.29606692836610704</v>
-      </c>
-      <c r="M37" s="52">
-        <f t="shared" si="3"/>
-        <v>0.38903674037484154</v>
+        <v>0.28551113720631677</v>
       </c>
       <c r="N37" s="28"/>
       <c r="O37" s="28"/>
@@ -6381,13 +6381,13 @@
         <f t="shared" si="0"/>
         <v>13468.375999999998</v>
       </c>
-      <c r="L38" s="50">
+      <c r="L38" s="40">
+        <f t="shared" si="1"/>
+        <v>0.29603190466319029</v>
+      </c>
+      <c r="M38" s="42">
         <f t="shared" si="2"/>
-        <v>0.29603190466319029</v>
-      </c>
-      <c r="M38" s="52">
-        <f t="shared" si="3"/>
-        <v>0.43876952945180625</v>
+        <v>0.33773448261319705</v>
       </c>
       <c r="N38" s="28"/>
       <c r="O38" s="28"/>
@@ -6435,13 +6435,13 @@
         <f t="shared" si="0"/>
         <v>12915.285</v>
       </c>
-      <c r="L39" s="50">
+      <c r="L39" s="40">
+        <f t="shared" si="1"/>
+        <v>0.29376572022994463</v>
+      </c>
+      <c r="M39" s="42">
         <f t="shared" si="2"/>
-        <v>0.29376572022994463</v>
-      </c>
-      <c r="M39" s="52">
-        <f t="shared" si="3"/>
-        <v>0.44854488305910406</v>
+        <v>0.3565140838936191</v>
       </c>
       <c r="N39" s="28"/>
       <c r="O39" s="28"/>
@@ -6489,13 +6489,13 @@
         <f t="shared" si="0"/>
         <v>11690.712</v>
       </c>
-      <c r="L40" s="50">
+      <c r="L40" s="40">
+        <f t="shared" si="1"/>
+        <v>0.31556769168550214</v>
+      </c>
+      <c r="M40" s="42">
         <f t="shared" si="2"/>
-        <v>0.31556769168550214</v>
-      </c>
-      <c r="M40" s="52">
-        <f t="shared" si="3"/>
-        <v>0.41815442891758853</v>
+        <v>0.32726013608067667</v>
       </c>
       <c r="N40" s="28"/>
       <c r="O40" s="28"/>
@@ -6543,13 +6543,13 @@
         <f t="shared" si="0"/>
         <v>11793.242</v>
       </c>
-      <c r="L41" s="50">
+      <c r="L41" s="40">
+        <f t="shared" si="1"/>
+        <v>0.32390457178780863</v>
+      </c>
+      <c r="M41" s="42">
         <f t="shared" si="2"/>
-        <v>0.32390457178780863</v>
-      </c>
-      <c r="M41" s="52">
-        <f t="shared" si="3"/>
-        <v>0.43269781117016004</v>
+        <v>0.34894289458318589</v>
       </c>
       <c r="N41" s="28"/>
       <c r="O41" s="28"/>
@@ -6597,13 +6597,13 @@
         <f t="shared" si="0"/>
         <v>11436.192000000001</v>
       </c>
-      <c r="L42" s="50">
+      <c r="L42" s="40">
+        <f t="shared" si="1"/>
+        <v>0.34407948030253427</v>
+      </c>
+      <c r="M42" s="42">
         <f t="shared" si="2"/>
-        <v>0.34407948030253427</v>
-      </c>
-      <c r="M42" s="52">
-        <f t="shared" si="3"/>
-        <v>0.41272575696525549</v>
+        <v>0.3295988734711694</v>
       </c>
       <c r="N42" s="28"/>
       <c r="O42" s="28"/>
@@ -6651,13 +6651,13 @@
         <f t="shared" si="0"/>
         <v>10597.955000000002</v>
       </c>
-      <c r="L43" s="50">
+      <c r="L43" s="40">
+        <f t="shared" si="1"/>
+        <v>0.37565351051216955</v>
+      </c>
+      <c r="M43" s="42">
         <f t="shared" si="2"/>
-        <v>0.37565351051216955</v>
-      </c>
-      <c r="M43" s="52">
-        <f t="shared" si="3"/>
-        <v>0.40316183641089237</v>
+        <v>0.31261446194100645</v>
       </c>
       <c r="N43" s="28"/>
       <c r="O43" s="28"/>
@@ -6705,13 +6705,13 @@
         <f t="shared" si="0"/>
         <v>9858.7780000000002</v>
       </c>
-      <c r="L44" s="50">
+      <c r="L44" s="40">
+        <f t="shared" si="1"/>
+        <v>0.41184769552575379</v>
+      </c>
+      <c r="M44" s="42">
         <f t="shared" si="2"/>
-        <v>0.41184769552575379</v>
-      </c>
-      <c r="M44" s="52">
-        <f t="shared" si="3"/>
-        <v>0.38948143471736552</v>
+        <v>0.30770770981961454</v>
       </c>
       <c r="N44" s="28"/>
       <c r="O44" s="28"/>
@@ -6753,13 +6753,13 @@
         <f>SUM(C45:J45)</f>
         <v>9240.8330000000005</v>
       </c>
-      <c r="L45" s="50">
+      <c r="L45" s="40">
+        <f t="shared" si="1"/>
+        <v>0.45768720200873664</v>
+      </c>
+      <c r="M45" s="42">
         <f t="shared" si="2"/>
-        <v>0.45768720200873664</v>
-      </c>
-      <c r="M45" s="52">
-        <f t="shared" si="3"/>
-        <v>0.34604034073551593</v>
+        <v>0.26061633188263439</v>
       </c>
       <c r="N45" s="28"/>
       <c r="O45" s="28"/>
@@ -6801,13 +6801,13 @@
         <f t="shared" si="0"/>
         <v>9448.5859999999993</v>
       </c>
-      <c r="L46" s="50">
+      <c r="L46" s="40">
+        <f t="shared" si="1"/>
+        <v>0.47866379159802325</v>
+      </c>
+      <c r="M46" s="42">
         <f t="shared" si="2"/>
-        <v>0.47866379159802325</v>
-      </c>
-      <c r="M46" s="52">
-        <f t="shared" si="3"/>
-        <v>0.32127505639468174</v>
+        <v>0.23370989055928582</v>
       </c>
       <c r="N46" s="28"/>
       <c r="O46" s="28"/>
@@ -6849,13 +6849,13 @@
         <f t="shared" si="0"/>
         <v>10055.264999999999</v>
       </c>
-      <c r="L47" s="50">
+      <c r="L47" s="40">
+        <f t="shared" si="1"/>
+        <v>0.44247297311408501</v>
+      </c>
+      <c r="M47" s="42">
         <f t="shared" si="2"/>
-        <v>0.44247297311408501</v>
-      </c>
-      <c r="M47" s="52">
-        <f t="shared" si="3"/>
-        <v>0.34433741925250105</v>
+        <v>0.26514089882265657</v>
       </c>
       <c r="N47" s="28"/>
       <c r="O47" s="28"/>
@@ -6897,13 +6897,13 @@
         <f t="shared" si="0"/>
         <v>10144.219999999999</v>
       </c>
-      <c r="L48" s="50">
+      <c r="L48" s="40">
+        <f t="shared" si="1"/>
+        <v>0.46694620187653663</v>
+      </c>
+      <c r="M48" s="42">
         <f t="shared" si="2"/>
-        <v>0.46694620187653663</v>
-      </c>
-      <c r="M48" s="52">
-        <f t="shared" si="3"/>
-        <v>0.3105994349491632</v>
+        <v>0.2441657416735836</v>
       </c>
       <c r="N48" s="28"/>
       <c r="O48" s="28"/>
@@ -6942,16 +6942,16 @@
         <v>1668.2600000000002</v>
       </c>
       <c r="K49" s="27">
-        <f t="shared" ref="K49" si="4">SUM(C49:J49)</f>
+        <f t="shared" ref="K49" si="3">SUM(C49:J49)</f>
         <v>9942.9350000000013</v>
       </c>
-      <c r="L49" s="50">
+      <c r="L49" s="40">
+        <f t="shared" si="1"/>
+        <v>0.50400299308001106</v>
+      </c>
+      <c r="M49" s="42">
         <f t="shared" si="2"/>
-        <v>0.50400299308001106</v>
-      </c>
-      <c r="M49" s="52">
-        <f t="shared" si="3"/>
-        <v>0.27578225141771512</v>
+        <v>0.21685699443876474</v>
       </c>
       <c r="N49" s="28"/>
       <c r="O49" s="28"/>
@@ -6990,16 +6990,16 @@
         <v>1870.0140000000001</v>
       </c>
       <c r="K50" s="15">
-        <f t="shared" ref="K50" si="5">SUM(C50:J50)</f>
+        <f t="shared" ref="K50" si="4">SUM(C50:J50)</f>
         <v>9093.2000000000007</v>
       </c>
-      <c r="L50" s="50">
+      <c r="L50" s="40">
+        <f t="shared" si="1"/>
+        <v>0.55759358641622303</v>
+      </c>
+      <c r="M50" s="42">
         <f t="shared" si="2"/>
-        <v>0.55759358641622303</v>
-      </c>
-      <c r="M50" s="52">
-        <f t="shared" si="3"/>
-        <v>0.19931069370518628</v>
+        <v>0.18918994413407822</v>
       </c>
       <c r="N50" s="28"/>
       <c r="O50" s="28"/>
@@ -7038,15 +7038,15 @@
         <v>1560.0740000000005</v>
       </c>
       <c r="K51" s="33">
-        <f t="shared" ref="K51" si="6">SUM(C51:J51)</f>
+        <f t="shared" ref="K51" si="5">SUM(C51:J51)</f>
         <v>7858.6537500000004</v>
       </c>
-      <c r="L51" s="50">
+      <c r="L51" s="40">
+        <f t="shared" si="1"/>
+        <v>0.62005785660171109</v>
+      </c>
+      <c r="M51" s="42">
         <f t="shared" si="2"/>
-        <v>0.62005785660171109</v>
-      </c>
-      <c r="M51" s="52">
-        <f t="shared" si="3"/>
         <v>0.15887069079739008</v>
       </c>
       <c r="N51" s="28"/>
@@ -7089,12 +7089,12 @@
         <f t="shared" si="0"/>
         <v>8475</v>
       </c>
-      <c r="L52" s="50">
+      <c r="L52" s="40">
+        <f t="shared" si="1"/>
+        <v>0.59598820058997048</v>
+      </c>
+      <c r="M52" s="42">
         <f t="shared" si="2"/>
-        <v>0.59598820058997048</v>
-      </c>
-      <c r="M52" s="52">
-        <f t="shared" si="3"/>
         <v>0.17427728613569321</v>
       </c>
       <c r="N52" s="28"/>
@@ -7139,12 +7139,12 @@
         <f t="shared" si="0"/>
         <v>8328</v>
       </c>
-      <c r="L53" s="50">
+      <c r="L53" s="40">
+        <f t="shared" si="1"/>
+        <v>0.62115754082612873</v>
+      </c>
+      <c r="M53" s="42">
         <f t="shared" si="2"/>
-        <v>0.62115754082612873</v>
-      </c>
-      <c r="M53" s="52">
-        <f t="shared" si="3"/>
         <v>0.13076368876080691</v>
       </c>
       <c r="N53" s="28"/>
@@ -7189,13 +7189,13 @@
         <f t="shared" si="0"/>
         <v>8700</v>
       </c>
-      <c r="L54" s="50">
+      <c r="L54" s="40">
+        <f t="shared" si="1"/>
+        <v>0.61057471264367813</v>
+      </c>
+      <c r="M54" s="42">
         <f t="shared" si="2"/>
-        <v>0.61057471264367813</v>
-      </c>
-      <c r="M54" s="52">
-        <f t="shared" si="3"/>
-        <v>0.13666666666666666</v>
+        <v>0.12229885057471264</v>
       </c>
       <c r="N54" s="28"/>
       <c r="O54" s="28"/>
@@ -7209,18 +7209,18 @@
       <c r="B55" s="16"/>
     </row>
     <row r="56" spans="2:26" ht="15" customHeight="1">
-      <c r="B56" s="45" t="s">
+      <c r="B56" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="45"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="45"/>
+      <c r="C56" s="49"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="49"/>
+      <c r="J56" s="49"/>
+      <c r="K56" s="49"/>
       <c r="L56" s="4"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
@@ -7237,18 +7237,18 @@
       <c r="Z56" s="4"/>
     </row>
     <row r="57" spans="2:26" ht="28.5" customHeight="1">
-      <c r="B57" s="44" t="s">
+      <c r="B57" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
-      <c r="F57" s="44"/>
-      <c r="G57" s="44"/>
-      <c r="H57" s="44"/>
-      <c r="I57" s="44"/>
-      <c r="J57" s="44"/>
-      <c r="K57" s="44"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
+      <c r="F57" s="48"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="48"/>
+      <c r="I57" s="48"/>
+      <c r="J57" s="48"/>
+      <c r="K57" s="48"/>
       <c r="L57" s="3"/>
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
@@ -7265,32 +7265,32 @@
       <c r="Z57" s="3"/>
     </row>
     <row r="58" spans="2:26">
-      <c r="B58" s="46" t="s">
+      <c r="B58" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="40"/>
-      <c r="K58" s="40"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44"/>
+      <c r="E58" s="44"/>
+      <c r="F58" s="44"/>
+      <c r="G58" s="44"/>
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44"/>
+      <c r="K58" s="44"/>
     </row>
     <row r="59" spans="2:26" ht="43.35" customHeight="1">
-      <c r="B59" s="45" t="s">
+      <c r="B59" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="45"/>
-      <c r="J59" s="45"/>
-      <c r="K59" s="45"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="49"/>
     </row>
     <row r="60" spans="2:26">
       <c r="B60" s="1" t="s">
@@ -7298,46 +7298,46 @@
       </c>
     </row>
     <row r="61" spans="2:26">
-      <c r="B61" s="40" t="s">
+      <c r="B61" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C61" s="40"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="40"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40"/>
-      <c r="I61" s="40"/>
-      <c r="J61" s="40"/>
-      <c r="K61" s="40"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="44"/>
     </row>
     <row r="63" spans="2:26">
-      <c r="B63" s="40" t="s">
+      <c r="B63" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="40"/>
-      <c r="D63" s="40"/>
-      <c r="E63" s="40"/>
-      <c r="F63" s="40"/>
-      <c r="G63" s="40"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="40"/>
-      <c r="K63" s="40"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="44"/>
+      <c r="H63" s="44"/>
+      <c r="I63" s="44"/>
+      <c r="J63" s="44"/>
+      <c r="K63" s="44"/>
     </row>
     <row r="64" spans="2:26">
-      <c r="B64" s="40" t="s">
+      <c r="B64" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="40"/>
-      <c r="D64" s="40"/>
-      <c r="E64" s="40"/>
-      <c r="F64" s="40"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="40"/>
-      <c r="I64" s="40"/>
-      <c r="J64" s="40"/>
-      <c r="K64" s="40"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="44"/>
+      <c r="G64" s="44"/>
+      <c r="H64" s="44"/>
+      <c r="I64" s="44"/>
+      <c r="J64" s="44"/>
+      <c r="K64" s="44"/>
     </row>
     <row r="65" spans="2:2" ht="15">
       <c r="B65" s="2"/>
@@ -7391,17 +7391,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="13.5" thickBot="1"/>
     <row r="2" spans="2:10" ht="39" customHeight="1" thickBot="1">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
     </row>
     <row r="3" spans="2:10" ht="40.5" customHeight="1">
       <c r="B3" s="9" t="s">
@@ -8920,21 +8920,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C64A56E9F85AC84187966BAEAF7CF07F" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ebe467e1bc15984d42e81a614a86359f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1b167cac-9da6-43f0-b7e7-4775de4a2f66" xmlns:ns3="9073c3f8-2855-48ea-b895-d99d76b52c59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="41a20adf9409c19ba3f46e581422b7df" ns2:_="" ns3:_="">
     <xsd:import namespace="1b167cac-9da6-43f0-b7e7-4775de4a2f66"/>
@@ -9105,32 +9090,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ABB01B9-6CF5-49B4-948F-049867CFC202}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="9073c3f8-2855-48ea-b895-d99d76b52c59"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1b167cac-9da6-43f0-b7e7-4775de4a2f66"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87E190B9-0F89-45BF-9D09-0F1682592553}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0595E14-2145-48DD-997B-880510EB1042}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9147,4 +9122,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87E190B9-0F89-45BF-9D09-0F1682592553}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0ABB01B9-6CF5-49B4-948F-049867CFC202}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="9073c3f8-2855-48ea-b895-d99d76b52c59"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1b167cac-9da6-43f0-b7e7-4775de4a2f66"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>